<commit_message>
added meta data files and added LLC field to surveys
</commit_message>
<xml_diff>
--- a/Tables for data for each city/Tables for Each City.xlsx
+++ b/Tables for data for each city/Tables for Each City.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8chas\Documents\CURO-GICH-\Tables for data for each city\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B41B62-4B6D-4A3A-B3C8-EE3B788B5DCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F9C6CE-03ED-400A-97AF-1562EF216F7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Warrenton" sheetId="1" r:id="rId1"/>
@@ -24833,7 +24833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
@@ -25121,7 +25121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D364D1B-B80D-4395-A5C9-D27C70B1D956}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1:U4"/>
     </sheetView>
   </sheetViews>

</xml_diff>